<commit_message>
SHell commonds part 1
</commit_message>
<xml_diff>
--- a/git_commands.xlsx
+++ b/git_commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g-jiuzhou\Desktop\git-commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EEA496-FBEC-4621-AE47-93E3E67FFECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E2328F-7BCF-4C87-B95F-7C95970BB614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52125" yWindow="-25335" windowWidth="29040" windowHeight="17640" xr2:uid="{21F98F57-BB0F-4528-B4A7-F94A878569B3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Command</t>
   </si>
@@ -95,6 +95,57 @@
   </si>
   <si>
     <t>touch file1.txt</t>
+  </si>
+  <si>
+    <t>git rm</t>
+  </si>
+  <si>
+    <t>git rm file1.txt</t>
+  </si>
+  <si>
+    <t>remove a file from the filesystem</t>
+  </si>
+  <si>
+    <t>git rm --cached</t>
+  </si>
+  <si>
+    <t>git rm --cached  file1.txt</t>
+  </si>
+  <si>
+    <t>remove a file from the git repository, but not from the filesystem. File becomes untracked</t>
+  </si>
+  <si>
+    <t>echo "Hello, world"</t>
+  </si>
+  <si>
+    <t>echo "content to write to file" &gt; file_name.txt</t>
+  </si>
+  <si>
+    <t>write the content to the file, create the file at the mean time</t>
+  </si>
+  <si>
+    <t>echo "hello world" &gt; another-file.txt</t>
+  </si>
+  <si>
+    <t>ls</t>
+  </si>
+  <si>
+    <t>list files in a folder</t>
+  </si>
+  <si>
+    <t>ls -la</t>
+  </si>
+  <si>
+    <t>list files in a folder, including hiden ones</t>
+  </si>
+  <si>
+    <t>cat file_name</t>
+  </si>
+  <si>
+    <t>print the content of the file in the termimal</t>
+  </si>
+  <si>
+    <t>cat another-file.txt</t>
   </si>
 </sst>
 </file>
@@ -455,19 +506,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1528F407-7F66-41A7-84A5-F18FCB6516A9}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.1796875" customWidth="1"/>
-    <col min="2" max="2" width="30.36328125" customWidth="1"/>
+    <col min="2" max="2" width="79.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -513,6 +564,9 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -545,6 +599,66 @@
       </c>
       <c r="C8" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shell command part 2
</commit_message>
<xml_diff>
--- a/git_commands.xlsx
+++ b/git_commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g-jiuzhou\Desktop\git-commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E2328F-7BCF-4C87-B95F-7C95970BB614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67101246-11F7-4F9C-8480-9ECBC602D523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52125" yWindow="-25335" windowWidth="29040" windowHeight="17640" xr2:uid="{21F98F57-BB0F-4528-B4A7-F94A878569B3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Command</t>
   </si>
@@ -146,6 +146,33 @@
   </si>
   <si>
     <t>cat another-file.txt</t>
+  </si>
+  <si>
+    <t>echo &gt;&gt;</t>
+  </si>
+  <si>
+    <t>attach content to a file</t>
+  </si>
+  <si>
+    <t>echo "Another line" &gt;&gt; another-file.txt</t>
+  </si>
+  <si>
+    <t>nano new-file.txt</t>
+  </si>
+  <si>
+    <t>rm</t>
+  </si>
+  <si>
+    <t>rm new-file.txt</t>
+  </si>
+  <si>
+    <t>remove files</t>
+  </si>
+  <si>
+    <t>directories</t>
+  </si>
+  <si>
+    <t>rm -rf new-folder</t>
   </si>
 </sst>
 </file>
@@ -506,13 +533,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1528F407-7F66-41A7-84A5-F18FCB6516A9}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -556,6 +583,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -659,6 +689,39 @@
       </c>
       <c r="C14" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Basic Git Operations 48-62
</commit_message>
<xml_diff>
--- a/git_commands.xlsx
+++ b/git_commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g-jiuzhou\Desktop\git-commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67101246-11F7-4F9C-8480-9ECBC602D523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B91096-A0E3-46C7-B92B-913A5105717E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52125" yWindow="-25335" windowWidth="29040" windowHeight="17640" xr2:uid="{21F98F57-BB0F-4528-B4A7-F94A878569B3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
   <si>
     <t>Command</t>
   </si>
@@ -130,9 +130,6 @@
     <t>ls</t>
   </si>
   <si>
-    <t>list files in a folder</t>
-  </si>
-  <si>
     <t>ls -la</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>cat file_name</t>
   </si>
   <si>
-    <t>print the content of the file in the termimal</t>
-  </si>
-  <si>
     <t>cat another-file.txt</t>
   </si>
   <si>
@@ -173,6 +167,105 @@
   </si>
   <si>
     <t>rm -rf new-folder</t>
+  </si>
+  <si>
+    <t>git init</t>
+  </si>
+  <si>
+    <t>initialize a folder as a repository, need to move to the folder using cd folder-name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start . </t>
+  </si>
+  <si>
+    <t>open windows exporer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">explorer . </t>
+  </si>
+  <si>
+    <t>print the content of the file in the termimal, can see file content in .git folder in a repos</t>
+  </si>
+  <si>
+    <t>git hash-object</t>
+  </si>
+  <si>
+    <t>git cat-file</t>
+  </si>
+  <si>
+    <t>git mktree</t>
+  </si>
+  <si>
+    <t>create sha1 hash of an object</t>
+  </si>
+  <si>
+    <t>echo "Hello, Git" | git hash-object --stdin -w</t>
+  </si>
+  <si>
+    <t>With -stdin, standard input, it will print the Sha1 hash in the termianl, with opention w, the has will be write into objects folder in .git</t>
+  </si>
+  <si>
+    <t>Example note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">options -p/-s/-t will show content/size/type of the object </t>
+  </si>
+  <si>
+    <t>will show the content of the SHA1-hash</t>
+  </si>
+  <si>
+    <t>git cat-file -p SHA1-hash</t>
+  </si>
+  <si>
+    <t>git hash-object new-file.txt -w</t>
+  </si>
+  <si>
+    <t>write the SHA1 hash into the object folder. If without option -w, the SHA1 hash will be printed in the terminal</t>
+  </si>
+  <si>
+    <t>shasum</t>
+  </si>
+  <si>
+    <t>create SHA1 hash using the git object type, size, delimiter and contenet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> echo -e "blob 30\0Second file in Git repository" | shasum</t>
+  </si>
+  <si>
+    <t>will get SHA1 hash: 4400aae52a27341314f423095846b1f215a7cf08</t>
+  </si>
+  <si>
+    <t>git ls-files</t>
+  </si>
+  <si>
+    <t>list files in the staging area</t>
+  </si>
+  <si>
+    <t>git ls-files -s</t>
+  </si>
+  <si>
+    <t>will show in a table format</t>
+  </si>
+  <si>
+    <t>git readtree</t>
+  </si>
+  <si>
+    <t>retrieve files from repository and put them in the staging area</t>
+  </si>
+  <si>
+    <t>git checkout-index -a</t>
+  </si>
+  <si>
+    <t>reading all files from staging area into working directory</t>
+  </si>
+  <si>
+    <t>find .git/objects -type f</t>
+  </si>
+  <si>
+    <t>find file type objects in the repository</t>
+  </si>
+  <si>
+    <t>list files in a folder, or in the working directory in a repository</t>
   </si>
 </sst>
 </file>
@@ -533,13 +626,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1528F407-7F66-41A7-84A5-F18FCB6516A9}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,7 +642,7 @@
     <col min="3" max="3" width="50.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -559,8 +652,11 @@
       <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -568,7 +664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -576,7 +672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -584,10 +680,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -598,7 +694,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -609,7 +705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -620,7 +716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -631,7 +727,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -642,7 +738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -653,7 +749,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -664,64 +760,195 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B18" t="s">
         <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1048576" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B1048576" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Git Branches and HEAD 63-79
</commit_message>
<xml_diff>
--- a/git_commands.xlsx
+++ b/git_commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g-jiuzhou\Desktop\git-commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B91096-A0E3-46C7-B92B-913A5105717E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FC803D-E2E0-4032-9016-96A05ACF97F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52125" yWindow="-25335" windowWidth="29040" windowHeight="17640" xr2:uid="{21F98F57-BB0F-4528-B4A7-F94A878569B3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
   <si>
     <t>Command</t>
   </si>
@@ -266,6 +266,66 @@
   </si>
   <si>
     <t>list files in a folder, or in the working directory in a repository</t>
+  </si>
+  <si>
+    <t>git checkout</t>
+  </si>
+  <si>
+    <t>checkout to different branch or commit</t>
+  </si>
+  <si>
+    <t>cat .git/HEAD</t>
+  </si>
+  <si>
+    <t>to see which SHA1 hash the HEAD is pointing</t>
+  </si>
+  <si>
+    <t>cat .git/refs/heads/main</t>
+  </si>
+  <si>
+    <t>to check the SHA1 hash of the last commit of the main branch</t>
+  </si>
+  <si>
+    <t>list all local branches</t>
+  </si>
+  <si>
+    <t>git branch</t>
+  </si>
+  <si>
+    <t>git branch branch_name</t>
+  </si>
+  <si>
+    <t>create a new branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git checkout branch_name </t>
+  </si>
+  <si>
+    <t>checkout specific branch</t>
+  </si>
+  <si>
+    <t>git branch -d branch_name</t>
+  </si>
+  <si>
+    <t>git branch -m old_branch_name new_branch_name</t>
+  </si>
+  <si>
+    <t>rename old_branch_name as new_branch_name</t>
+  </si>
+  <si>
+    <t>delete branch branch_name, but only to delete merged branch. If you ang to delete non-merged branch, use -D option</t>
+  </si>
+  <si>
+    <t>git branch -D branch_name</t>
+  </si>
+  <si>
+    <t>Force to delete the branch even it is not merged.</t>
+  </si>
+  <si>
+    <t>git checkout -b branch_name</t>
+  </si>
+  <si>
+    <t>create new branch, and checkout it</t>
   </si>
 </sst>
 </file>
@@ -632,12 +692,12 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.1796875" customWidth="1"/>
+    <col min="1" max="1" width="45.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.6328125" customWidth="1"/>
   </cols>
@@ -946,6 +1006,84 @@
         <v>75</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B1048576" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Cloning exploring and modifying public repositories 80-89
</commit_message>
<xml_diff>
--- a/git_commands.xlsx
+++ b/git_commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g-jiuzhou\Desktop\git-commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FC803D-E2E0-4032-9016-96A05ACF97F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8371B72E-AABD-4EED-8C19-464842EBDE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52125" yWindow="-25335" windowWidth="29040" windowHeight="17640" xr2:uid="{21F98F57-BB0F-4528-B4A7-F94A878569B3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
   <si>
     <t>Command</t>
   </si>
@@ -326,6 +326,39 @@
   </si>
   <si>
     <t>create new branch, and checkout it</t>
+  </si>
+  <si>
+    <t>clone a public remote repository</t>
+  </si>
+  <si>
+    <t>git clone https://github.com/wangjiuzhou100/git-commands.git</t>
+  </si>
+  <si>
+    <t>git unpack-objects</t>
+  </si>
+  <si>
+    <t>unpack the packed objects in the folder .git/pack, with the suffix .pack</t>
+  </si>
+  <si>
+    <t>cat name-of-the-packed-file | git unpack-objects</t>
+  </si>
+  <si>
+    <t>Should go to the .git folder to run the command. The pack file should be copied to the .git folder and deleted from the .git/objects/pack folder</t>
+  </si>
+  <si>
+    <t>git diff</t>
+  </si>
+  <si>
+    <t>see the difference of changes</t>
+  </si>
+  <si>
+    <t>The difference shows covers some lines not changed. For example, @@ -6,11 +6,13 @@ , -6 is from line 6 of the former version, and 6 means the modified file is also to start line 6. So line 6 and maybe more lines are common lines. 11 is to counter 11 lines from line 6 for the previous version, wihle count 13 lines for the current version. And the changed is between the lines with colors.</t>
+  </si>
+  <si>
+    <t>git commit -m "commit information" -a</t>
+  </si>
+  <si>
+    <t>first add all  changes to the staging area, and then commit</t>
   </si>
 </sst>
 </file>
@@ -689,15 +722,15 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.6328125" customWidth="1"/>
   </cols>
@@ -1084,6 +1117,50 @@
         <v>96</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B1048576" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Section 7 to Section 10-130
</commit_message>
<xml_diff>
--- a/git_commands.xlsx
+++ b/git_commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g-jiuzhou\Desktop\git-commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8371B72E-AABD-4EED-8C19-464842EBDE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D452E9B6-9317-4D6C-8BB0-9345DD3CDF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52125" yWindow="-25335" windowWidth="29040" windowHeight="17640" xr2:uid="{21F98F57-BB0F-4528-B4A7-F94A878569B3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="147">
   <si>
     <t>Command</t>
   </si>
@@ -359,13 +359,130 @@
   </si>
   <si>
     <t>first add all  changes to the staging area, and then commit</t>
+  </si>
+  <si>
+    <t>git merge Branch_To_Merge</t>
+  </si>
+  <si>
+    <t>Merge the Branch_To_Merge into the checkouted branch</t>
+  </si>
+  <si>
+    <t>git merge feature-1</t>
+  </si>
+  <si>
+    <t>reset the head to the SHA1-hash</t>
+  </si>
+  <si>
+    <t>git reset --hard SHA1-hash</t>
+  </si>
+  <si>
+    <t>can cancel a merge by setting the SHA1-hash as the one before meerge. NOTE, this is not reversible.</t>
+  </si>
+  <si>
+    <t>For example, if you want to merge feature-1 into the main branch, you need to first checkout main branch. If it is fast forward merge, nothing will pop up. If it is 3-way merge, it will pop out the editor to into the reason to merge.</t>
+  </si>
+  <si>
+    <t>git merge --abort</t>
+  </si>
+  <si>
+    <t>to abort a merge which has merge conflict</t>
+  </si>
+  <si>
+    <t>You can put -a options as: git commit -a -m "commit information"</t>
+  </si>
+  <si>
+    <t>git remote</t>
+  </si>
+  <si>
+    <t>list all remote servers to your local repositories</t>
+  </si>
+  <si>
+    <t>the default remote server name is origin, if you use git pull, it will pull from origin</t>
+  </si>
+  <si>
+    <t>git remote -v</t>
+  </si>
+  <si>
+    <t>verbose of git remote</t>
+  </si>
+  <si>
+    <t>you will see the name of the remote server and fetch and pull URLs</t>
+  </si>
+  <si>
+    <t>git branch -a</t>
+  </si>
+  <si>
+    <t>list all branches, including local and remote branches</t>
+  </si>
+  <si>
+    <t>git branch --all</t>
+  </si>
+  <si>
+    <t>options either -a or --all</t>
+  </si>
+  <si>
+    <t>git branch -r/git branch --remote</t>
+  </si>
+  <si>
+    <t>only show remote branches</t>
+  </si>
+  <si>
+    <t>When you clone a remote repository into your local reposiotory, only the default branch is cloned as the tracking reposiotory</t>
+  </si>
+  <si>
+    <t>git branch -vv</t>
+  </si>
+  <si>
+    <t>See tracking branches</t>
+  </si>
+  <si>
+    <t>feature-1 2a45690 [origin/feature-1] another local change: This is the info shows that feature-1 is tracking [origin/featrue-1],  the SHA1-hash is the last commit, and "Another local change" is the commit information of the last commit.</t>
+  </si>
+  <si>
+    <t>git checkout remote-branch-name</t>
+  </si>
+  <si>
+    <t>set local branch to track remote branch, even though the remote branch does not exist when you use git branch</t>
+  </si>
+  <si>
+    <t>If you create a branch with the same name as a remote branch, and then check out it, it will not track the remote branch.</t>
+  </si>
+  <si>
+    <t>git branch --set-upstream-to=origin/feature-y feature-y</t>
+  </si>
+  <si>
+    <t>set local branch feature-y to track remote branch origin/feature-y</t>
+  </si>
+  <si>
+    <t>git remote show remote-server-name</t>
+  </si>
+  <si>
+    <t>show the mapping of local branches tracking remote branches</t>
+  </si>
+  <si>
+    <t>git remote show origin</t>
+  </si>
+  <si>
+    <t>remote-server-name is origin. This command can show remote branch even it is not fetched and tracked. And it can also show that a deleted branch in the remote server disappears. While git branch -r does not show untracked branches</t>
+  </si>
+  <si>
+    <t>git remote prune origin</t>
+  </si>
+  <si>
+    <t>delete remote branch deleted in the remote server</t>
+  </si>
+  <si>
+    <t>git pull</t>
+  </si>
+  <si>
+    <t>update only single local currently checked out branch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +493,13 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -401,10 +525,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,10 +847,10 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1124,6 +1249,9 @@
       <c r="B39" t="s">
         <v>97</v>
       </c>
+      <c r="D39" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -1159,6 +1287,146 @@
       </c>
       <c r="B42" t="s">
         <v>107</v>
+      </c>
+      <c r="D42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>121</v>
+      </c>
+      <c r="B47" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B52" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" t="s">
+        <v>140</v>
+      </c>
+      <c r="C53" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>143</v>
+      </c>
+      <c r="B54" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
git fetch, push and pull to section 140
</commit_message>
<xml_diff>
--- a/git_commands.xlsx
+++ b/git_commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g-jiuzhou\Desktop\git-commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D452E9B6-9317-4D6C-8BB0-9345DD3CDF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A602EB0F-1B84-465D-AF62-37A75126AE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52125" yWindow="-25335" windowWidth="29040" windowHeight="17640" xr2:uid="{21F98F57-BB0F-4528-B4A7-F94A878569B3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="165">
   <si>
     <t>Command</t>
   </si>
@@ -476,6 +476,60 @@
   </si>
   <si>
     <t>update only single local currently checked out branch</t>
+  </si>
+  <si>
+    <t>During "git pull" Git will first execute "git fetch". After fetching it will update .git/FETCH_HEAD list and the first branch in this list will be currently checkedout branch. Finally, Git executes "git merge FETCH_HEAD" command that finds first branch in .git/fetch_HEAD list without "not-for-merge" tag and merges it into lcoal tracking currently checkout out branch.</t>
+  </si>
+  <si>
+    <t>git fetch -v</t>
+  </si>
+  <si>
+    <t>fetch changes from remote server, will create object in the local repository, but not merged in the staging area and working directory</t>
+  </si>
+  <si>
+    <t>git merge FETCH_HEAD</t>
+  </si>
+  <si>
+    <t>merge the fetched changes from server and merge with stating area and working directory</t>
+  </si>
+  <si>
+    <t>git push --set-upsteam origin local-branch-name</t>
+  </si>
+  <si>
+    <t>push a local branch which is absent in the remote server origin</t>
+  </si>
+  <si>
+    <t>git push -v -u origin local-branch-name</t>
+  </si>
+  <si>
+    <t>short version of --set-upstream</t>
+  </si>
+  <si>
+    <t>git remote update origin --prune</t>
+  </si>
+  <si>
+    <t>cancel of tracking deleted remote branch</t>
+  </si>
+  <si>
+    <t>git push origin -d remote-branch-name</t>
+  </si>
+  <si>
+    <t>delete remote branch remote-branch-name in the local terminal</t>
+  </si>
+  <si>
+    <t>git show-ref</t>
+  </si>
+  <si>
+    <t>show all the refereces -including local repository and remote server repository</t>
+  </si>
+  <si>
+    <t>git show-ref main</t>
+  </si>
+  <si>
+    <t>only show references of main -local and remote</t>
+  </si>
+  <si>
+    <t>You show the same for any other branches</t>
   </si>
 </sst>
 </file>
@@ -847,10 +901,10 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
+      <selection pane="bottomRight" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1428,6 +1482,79 @@
       <c r="B55" s="3" t="s">
         <v>146</v>
       </c>
+      <c r="C55" t="s">
+        <v>145</v>
+      </c>
+      <c r="D55" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>148</v>
+      </c>
+      <c r="B56" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>152</v>
+      </c>
+      <c r="B58" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>156</v>
+      </c>
+      <c r="B60" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>158</v>
+      </c>
+      <c r="B61" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>160</v>
+      </c>
+      <c r="B62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>162</v>
+      </c>
+      <c r="B63" t="s">
+        <v>163</v>
+      </c>
+      <c r="D63" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="1048576" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B1048576" t="s">

</xml_diff>